<commit_message>
* added table with benchmark scenes * added triangle count histograms * started explaining test scenes
</commit_message>
<xml_diff>
--- a/latex/spreadsheets/c_hist.xlsx
+++ b/latex/spreadsheets/c_hist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r13_enlight\branches\MeshExtraction\Demonstrator\g\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\master\latex\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="c-hist" sheetId="1" r:id="rId1"/>
@@ -582,38 +582,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -702,11 +671,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="189564176"/>
-        <c:axId val="189564568"/>
+        <c:axId val="246396008"/>
+        <c:axId val="246396400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189564176"/>
+        <c:axId val="246396008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -763,16 +732,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189564568"/>
+        <c:crossAx val="246396400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:tickMarkSkip val="1000"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189564568"/>
+        <c:axId val="246396400"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -830,7 +800,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189564176"/>
+        <c:crossAx val="246396008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -851,12 +821,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1439,16 +1404,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>75525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>94800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1736,7 +1701,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
* some improvements to image floating * fixed some overfull boxes * updated sizes in histogram spreadsheets
</commit_message>
<xml_diff>
--- a/latex/spreadsheets/c_hist.xlsx
+++ b/latex/spreadsheets/c_hist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="c-hist" sheetId="1" r:id="rId1"/>
@@ -671,11 +671,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="246396008"/>
-        <c:axId val="246396400"/>
+        <c:axId val="372707048"/>
+        <c:axId val="372705480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246396008"/>
+        <c:axId val="372707048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246396400"/>
+        <c:crossAx val="372705480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -742,7 +742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246396400"/>
+        <c:axId val="372705480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -800,7 +800,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246396008"/>
+        <c:crossAx val="372707048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -839,7 +839,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1410,10 +1410,10 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>75525</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>94800</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>178800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1701,7 +1701,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>